<commit_message>
Cambios mínimos en ponderación
</commit_message>
<xml_diff>
--- a/entregables2daInm/Creativity_DFMEA.xlsx
+++ b/entregables2daInm/Creativity_DFMEA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\SemestreI_Creativity\entregables2daInm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isra\Documents\Semestrei\SemestreI_Creativity\entregables2daInm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F5854D-1E71-4AAA-9795-FD890F75A0E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3805D79F-B600-4DF6-BCED-21260CF4A64B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FMEA" sheetId="1" r:id="rId1"/>
@@ -1162,204 +1162,204 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1703,8 +1703,8 @@
   </sheetPr>
   <dimension ref="A1:W451"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D37" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1737,19 +1737,19 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="104"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="122"/>
       <c r="G1" s="2"/>
       <c r="H1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="89"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="91"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="114"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="2"/>
@@ -1761,19 +1761,19 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="91"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="114"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="95"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="118"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="2"/>
@@ -1907,22 +1907,22 @@
     </row>
     <row r="6" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="41"/>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="123" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="91" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="78">
+      <c r="E6" s="86">
         <v>8</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="120">
+      <c r="G6" s="75">
         <v>10</v>
       </c>
       <c r="H6" s="23" t="s">
@@ -1931,7 +1931,7 @@
       <c r="I6" s="72">
         <v>3</v>
       </c>
-      <c r="J6" s="123">
+      <c r="J6" s="78">
         <f>E6*G6*I6</f>
         <v>240</v>
       </c>
@@ -1955,15 +1955,15 @@
     </row>
     <row r="7" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="47"/>
-      <c r="B7" s="118"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="79"/>
+      <c r="B7" s="124"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="120">
-        <v>10</v>
+      <c r="G7" s="75">
+        <v>9</v>
       </c>
       <c r="H7" s="23" t="s">
         <v>92</v>
@@ -1971,9 +1971,9 @@
       <c r="I7" s="7">
         <v>8</v>
       </c>
-      <c r="J7" s="123">
+      <c r="J7" s="78">
         <f>$E$6*G7*I7</f>
-        <v>640</v>
+        <v>576</v>
       </c>
       <c r="K7" s="44"/>
       <c r="L7" s="23"/>
@@ -1989,28 +1989,28 @@
     </row>
     <row r="8" spans="1:18" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47"/>
-      <c r="B8" s="118"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="116" t="s">
+      <c r="B8" s="124"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="96">
+      <c r="G8" s="82">
         <v>5</v>
       </c>
-      <c r="H8" s="116" t="s">
+      <c r="H8" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="I8" s="78">
+      <c r="I8" s="86">
         <v>8</v>
       </c>
-      <c r="J8" s="124">
+      <c r="J8" s="89">
         <f>$E$6*G8*I8</f>
         <v>320</v>
       </c>
-      <c r="K8" s="84"/>
-      <c r="L8" s="96"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="82"/>
       <c r="M8" s="6"/>
       <c r="N8" s="45"/>
       <c r="O8" s="49"/>
@@ -2023,17 +2023,17 @@
     </row>
     <row r="9" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47"/>
-      <c r="B9" s="118"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="113"/>
-      <c r="G9" s="97"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="125"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="97"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="83"/>
       <c r="M9" s="6"/>
       <c r="N9" s="45"/>
       <c r="O9" s="21"/>
@@ -2046,14 +2046,14 @@
     </row>
     <row r="10" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47"/>
-      <c r="B10" s="118"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="80"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="121">
+      <c r="G10" s="76">
         <v>10</v>
       </c>
       <c r="H10" s="23" t="s">
@@ -2062,7 +2062,7 @@
       <c r="I10" s="7">
         <v>5</v>
       </c>
-      <c r="J10" s="123">
+      <c r="J10" s="78">
         <f>$E$6*G10*I10</f>
         <v>400</v>
       </c>
@@ -2077,34 +2077,34 @@
     </row>
     <row r="11" spans="1:18" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="47"/>
-      <c r="B11" s="118"/>
-      <c r="C11" s="100" t="s">
+      <c r="B11" s="124"/>
+      <c r="C11" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="78">
+      <c r="E11" s="86">
         <v>8</v>
       </c>
-      <c r="F11" s="98" t="s">
+      <c r="F11" s="119" t="s">
         <v>82</v>
       </c>
-      <c r="G11" s="78">
+      <c r="G11" s="86">
         <v>10</v>
       </c>
-      <c r="H11" s="116" t="s">
+      <c r="H11" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="I11" s="78">
+      <c r="I11" s="86">
         <v>4</v>
       </c>
-      <c r="J11" s="124">
+      <c r="J11" s="89">
         <f>$E$11*G11*I11</f>
         <v>320</v>
       </c>
-      <c r="K11" s="84"/>
-      <c r="L11" s="96"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="82"/>
       <c r="M11" s="8"/>
       <c r="N11" s="53"/>
       <c r="O11" s="42">
@@ -2123,17 +2123,17 @@
     </row>
     <row r="12" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="47"/>
-      <c r="B12" s="118"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="125"/>
-      <c r="K12" s="85"/>
-      <c r="L12" s="97"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="83"/>
       <c r="M12" s="8"/>
       <c r="N12" s="55"/>
       <c r="O12" s="52"/>
@@ -2146,10 +2146,10 @@
     </row>
     <row r="13" spans="1:18" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47"/>
-      <c r="B13" s="118"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="80"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="88"/>
       <c r="F13" s="21" t="s">
         <v>83</v>
       </c>
@@ -2162,7 +2162,7 @@
       <c r="I13" s="7">
         <v>10</v>
       </c>
-      <c r="J13" s="126">
+      <c r="J13" s="79">
         <f>$E$11*G13*I13</f>
         <v>800</v>
       </c>
@@ -2180,14 +2180,14 @@
     </row>
     <row r="14" spans="1:18" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="47"/>
-      <c r="B14" s="118"/>
-      <c r="C14" s="100" t="s">
+      <c r="B14" s="124"/>
+      <c r="C14" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="78">
+      <c r="E14" s="86">
         <v>8</v>
       </c>
       <c r="F14" s="21" t="s">
@@ -2202,7 +2202,7 @@
       <c r="I14" s="7">
         <v>7</v>
       </c>
-      <c r="J14" s="126">
+      <c r="J14" s="79">
         <f>$E$14*G14*I14</f>
         <v>392</v>
       </c>
@@ -2226,10 +2226,10 @@
     </row>
     <row r="15" spans="1:18" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="47"/>
-      <c r="B15" s="118"/>
-      <c r="C15" s="101"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="79"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="87"/>
       <c r="F15" s="21" t="s">
         <v>87</v>
       </c>
@@ -2242,7 +2242,7 @@
       <c r="I15" s="7">
         <v>9</v>
       </c>
-      <c r="J15" s="126">
+      <c r="J15" s="79">
         <f>$E$14*G15*I15</f>
         <v>504</v>
       </c>
@@ -2257,10 +2257,10 @@
     </row>
     <row r="16" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="47"/>
-      <c r="B16" s="118"/>
-      <c r="C16" s="102"/>
-      <c r="D16" s="88"/>
-      <c r="E16" s="80"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="88"/>
       <c r="F16" s="23" t="s">
         <v>86</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="I16" s="7">
         <v>5</v>
       </c>
-      <c r="J16" s="126">
+      <c r="J16" s="79">
         <f>$E$14*G16*I16</f>
         <v>240</v>
       </c>
@@ -2291,14 +2291,14 @@
     </row>
     <row r="17" spans="1:18" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="47"/>
-      <c r="B17" s="118"/>
-      <c r="C17" s="100" t="s">
+      <c r="B17" s="124"/>
+      <c r="C17" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="86" t="s">
+      <c r="D17" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="84">
+      <c r="E17" s="80">
         <v>8</v>
       </c>
       <c r="F17" s="57" t="s">
@@ -2313,7 +2313,7 @@
       <c r="I17" s="7">
         <v>5</v>
       </c>
-      <c r="J17" s="126">
+      <c r="J17" s="79">
         <f>$E$17*G17*I17</f>
         <v>200</v>
       </c>
@@ -2328,12 +2328,12 @@
     </row>
     <row r="18" spans="1:18" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="47"/>
-      <c r="B18" s="118"/>
-      <c r="C18" s="102"/>
-      <c r="D18" s="87" t="s">
+      <c r="B18" s="124"/>
+      <c r="C18" s="96"/>
+      <c r="D18" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="85"/>
+      <c r="E18" s="81"/>
       <c r="F18" s="57" t="s">
         <v>90</v>
       </c>
@@ -2346,7 +2346,7 @@
       <c r="I18" s="7">
         <v>3</v>
       </c>
-      <c r="J18" s="126">
+      <c r="J18" s="79">
         <f>$E$17*G18*I18</f>
         <v>120</v>
       </c>
@@ -2361,14 +2361,14 @@
     </row>
     <row r="19" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47"/>
-      <c r="B19" s="118"/>
-      <c r="C19" s="100" t="s">
+      <c r="B19" s="124"/>
+      <c r="C19" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="86" t="s">
+      <c r="D19" s="91" t="s">
         <v>129</v>
       </c>
-      <c r="E19" s="84">
+      <c r="E19" s="80">
         <v>7</v>
       </c>
       <c r="F19" s="44" t="s">
@@ -2383,7 +2383,7 @@
       <c r="I19" s="7">
         <v>8</v>
       </c>
-      <c r="J19" s="126">
+      <c r="J19" s="79">
         <f>$E$19*G19*I19</f>
         <v>448</v>
       </c>
@@ -2407,10 +2407,10 @@
     </row>
     <row r="20" spans="1:18" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="47"/>
-      <c r="B20" s="119"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="85"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="92"/>
+      <c r="E20" s="81"/>
       <c r="F20" s="54" t="s">
         <v>74</v>
       </c>
@@ -2423,7 +2423,7 @@
       <c r="I20" s="7">
         <v>8</v>
       </c>
-      <c r="J20" s="126">
+      <c r="J20" s="79">
         <f>$E$19*G20*I20</f>
         <v>504</v>
       </c>
@@ -2440,17 +2440,17 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105"/>
-      <c r="B21" s="81" t="s">
+      <c r="A21" s="107"/>
+      <c r="B21" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="91" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="86" t="s">
+      <c r="D21" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="78">
+      <c r="E21" s="86">
         <v>8</v>
       </c>
       <c r="F21" s="44" t="s">
@@ -2465,19 +2465,19 @@
       <c r="I21" s="7">
         <v>3</v>
       </c>
-      <c r="J21" s="126">
+      <c r="J21" s="79">
         <f>$E$21*G21*I21</f>
         <v>216</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="8"/>
-      <c r="N21" s="110"/>
-      <c r="O21" s="107">
+      <c r="N21" s="102"/>
+      <c r="O21" s="97">
         <f>E21</f>
         <v>8</v>
       </c>
-      <c r="P21" s="107">
+      <c r="P21" s="97">
         <f t="shared" ref="P21:P47" si="2">G21</f>
         <v>9</v>
       </c>
@@ -2488,11 +2488,11 @@
       </c>
     </row>
     <row r="22" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="106"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="80"/>
+      <c r="A22" s="108"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="88"/>
       <c r="F22" s="44" t="s">
         <v>113</v>
       </c>
@@ -2505,16 +2505,16 @@
       <c r="I22" s="7">
         <v>2</v>
       </c>
-      <c r="J22" s="126">
+      <c r="J22" s="79">
         <f>$E$21*G22*I22</f>
         <v>144</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="8"/>
-      <c r="N22" s="111"/>
-      <c r="O22" s="108"/>
-      <c r="P22" s="108"/>
+      <c r="N22" s="103"/>
+      <c r="O22" s="105"/>
+      <c r="P22" s="105"/>
       <c r="Q22" s="23"/>
       <c r="R22" s="46">
         <f t="shared" ref="R22:R30" si="3">O$21*P22*Q22</f>
@@ -2522,15 +2522,15 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="106"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="86" t="s">
+      <c r="A23" s="108"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="86" t="s">
+      <c r="D23" s="91" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="78">
+      <c r="E23" s="86">
         <v>10</v>
       </c>
       <c r="F23" s="44" t="s">
@@ -2545,16 +2545,16 @@
       <c r="I23" s="7">
         <v>2</v>
       </c>
-      <c r="J23" s="126">
+      <c r="J23" s="79">
         <f>$E$23*G23*I23</f>
         <v>200</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="8"/>
-      <c r="N23" s="111"/>
-      <c r="O23" s="108"/>
-      <c r="P23" s="108"/>
+      <c r="N23" s="103"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="105"/>
       <c r="Q23" s="23"/>
       <c r="R23" s="46">
         <f t="shared" si="3"/>
@@ -2562,11 +2562,11 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="106"/>
-      <c r="B24" s="82"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="80"/>
+      <c r="A24" s="108"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="88"/>
       <c r="F24" s="44" t="s">
         <v>113</v>
       </c>
@@ -2579,16 +2579,16 @@
       <c r="I24" s="7">
         <v>2</v>
       </c>
-      <c r="J24" s="126">
+      <c r="J24" s="79">
         <f>$E$23*G24*I24</f>
         <v>200</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="8"/>
-      <c r="N24" s="112"/>
-      <c r="O24" s="108"/>
-      <c r="P24" s="109"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="105"/>
+      <c r="P24" s="106"/>
       <c r="Q24" s="23"/>
       <c r="R24" s="46">
         <f t="shared" si="3"/>
@@ -2596,15 +2596,15 @@
       </c>
     </row>
     <row r="25" spans="1:18" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="106"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="86" t="s">
+      <c r="A25" s="108"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="75" t="s">
+      <c r="D25" s="110" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="78">
+      <c r="E25" s="86">
         <v>8</v>
       </c>
       <c r="F25" s="44" t="s">
@@ -2619,7 +2619,7 @@
       <c r="I25" s="7">
         <v>8</v>
       </c>
-      <c r="J25" s="126">
+      <c r="J25" s="79">
         <f>$E$25*G25*I25</f>
         <v>320</v>
       </c>
@@ -2633,15 +2633,15 @@
       <c r="R25" s="46"/>
     </row>
     <row r="26" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="106"/>
-      <c r="B26" s="82"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="80"/>
+      <c r="A26" s="108"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="88"/>
       <c r="F26" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="G26" s="122">
+      <c r="G26" s="77">
         <v>8</v>
       </c>
       <c r="H26" s="23" t="s">
@@ -2650,19 +2650,19 @@
       <c r="I26" s="7">
         <v>2</v>
       </c>
-      <c r="J26" s="126">
+      <c r="J26" s="79">
         <f>$E$25*G26*I26</f>
         <v>128</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="110"/>
-      <c r="O26" s="107">
+      <c r="N26" s="102"/>
+      <c r="O26" s="97">
         <f>E26</f>
         <v>0</v>
       </c>
-      <c r="P26" s="107">
+      <c r="P26" s="97">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -2673,21 +2673,21 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="106"/>
-      <c r="B27" s="82"/>
-      <c r="C27" s="75" t="s">
+      <c r="A27" s="108"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="110" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="D27" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="78">
+      <c r="E27" s="86">
         <v>8</v>
       </c>
       <c r="F27" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="G27" s="122">
+      <c r="G27" s="77">
         <v>7</v>
       </c>
       <c r="H27" s="23" t="s">
@@ -2696,29 +2696,29 @@
       <c r="I27" s="7">
         <v>3</v>
       </c>
-      <c r="J27" s="126">
+      <c r="J27" s="79">
         <f>$E$27*G27*I27</f>
         <v>168</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="8"/>
-      <c r="N27" s="111"/>
-      <c r="O27" s="108"/>
-      <c r="P27" s="108"/>
+      <c r="N27" s="103"/>
+      <c r="O27" s="105"/>
+      <c r="P27" s="105"/>
       <c r="Q27" s="23"/>
       <c r="R27" s="46"/>
     </row>
     <row r="28" spans="1:18" ht="49.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="106"/>
-      <c r="B28" s="82"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="80"/>
+      <c r="A28" s="108"/>
+      <c r="B28" s="100"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="88"/>
       <c r="F28" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="G28" s="122">
+      <c r="G28" s="77">
         <v>5</v>
       </c>
       <c r="H28" s="23" t="s">
@@ -2727,35 +2727,35 @@
       <c r="I28" s="7">
         <v>8</v>
       </c>
-      <c r="J28" s="126">
+      <c r="J28" s="79">
         <f>$E$27*G28*I28</f>
         <v>320</v>
       </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="8"/>
-      <c r="N28" s="111"/>
-      <c r="O28" s="108"/>
-      <c r="P28" s="108"/>
+      <c r="N28" s="103"/>
+      <c r="O28" s="105"/>
+      <c r="P28" s="105"/>
       <c r="Q28" s="23"/>
       <c r="R28" s="46"/>
     </row>
     <row r="29" spans="1:18" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="106"/>
-      <c r="B29" s="82"/>
-      <c r="C29" s="75" t="s">
+      <c r="A29" s="108"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="110" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="75" t="s">
+      <c r="D29" s="110" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="78">
+      <c r="E29" s="86">
         <v>10</v>
       </c>
       <c r="F29" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="G29" s="122">
+      <c r="G29" s="77">
         <v>4</v>
       </c>
       <c r="H29" s="23" t="s">
@@ -2764,29 +2764,29 @@
       <c r="I29" s="7">
         <v>9</v>
       </c>
-      <c r="J29" s="126">
+      <c r="J29" s="79">
         <f>$E$29*G29*I29</f>
         <v>360</v>
       </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="8"/>
-      <c r="N29" s="111"/>
-      <c r="O29" s="108"/>
-      <c r="P29" s="108"/>
+      <c r="N29" s="103"/>
+      <c r="O29" s="105"/>
+      <c r="P29" s="105"/>
       <c r="Q29" s="23"/>
       <c r="R29" s="46"/>
     </row>
     <row r="30" spans="1:18" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="114"/>
-      <c r="B30" s="83"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="80"/>
+      <c r="A30" s="109"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="111"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="88"/>
       <c r="F30" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="G30" s="122">
+      <c r="G30" s="77">
         <v>5</v>
       </c>
       <c r="H30" s="23" t="s">
@@ -2795,16 +2795,16 @@
       <c r="I30" s="7">
         <v>8</v>
       </c>
-      <c r="J30" s="126">
+      <c r="J30" s="79">
         <f>$E$29*G30*I30</f>
         <v>400</v>
       </c>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="8"/>
-      <c r="N30" s="112"/>
-      <c r="O30" s="113"/>
-      <c r="P30" s="109"/>
+      <c r="N30" s="104"/>
+      <c r="O30" s="85"/>
+      <c r="P30" s="106"/>
       <c r="Q30" s="23"/>
       <c r="R30" s="46">
         <f t="shared" si="3"/>
@@ -2814,19 +2814,19 @@
     <row r="31" spans="1:18" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="58"/>
       <c r="B31" s="59"/>
-      <c r="C31" s="86" t="s">
+      <c r="C31" s="91" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="75" t="s">
+      <c r="D31" s="110" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="78">
+      <c r="E31" s="86">
         <v>8</v>
       </c>
       <c r="F31" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="G31" s="122">
+      <c r="G31" s="77">
         <v>8</v>
       </c>
       <c r="H31" s="23" t="s">
@@ -2835,7 +2835,7 @@
       <c r="I31" s="73">
         <v>2</v>
       </c>
-      <c r="J31" s="126">
+      <c r="J31" s="79">
         <f>$E$31*G31*I31</f>
         <v>128</v>
       </c>
@@ -2851,13 +2851,13 @@
     <row r="32" spans="1:18" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="58"/>
       <c r="B32" s="59"/>
-      <c r="C32" s="87"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="79"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="126"/>
+      <c r="E32" s="87"/>
       <c r="F32" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="G32" s="122">
+      <c r="G32" s="77">
         <v>5</v>
       </c>
       <c r="H32" s="23" t="s">
@@ -2866,7 +2866,7 @@
       <c r="I32" s="73">
         <v>8</v>
       </c>
-      <c r="J32" s="126">
+      <c r="J32" s="79">
         <f>$E$31*G32*I32</f>
         <v>320</v>
       </c>
@@ -2880,13 +2880,13 @@
       <c r="R32" s="46"/>
     </row>
     <row r="33" spans="1:23" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="105"/>
-      <c r="B33" s="81" t="s">
+      <c r="A33" s="107"/>
+      <c r="B33" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="88"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="80"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="88"/>
       <c r="F33" s="23" t="s">
         <v>119</v>
       </c>
@@ -2899,15 +2899,15 @@
       <c r="I33" s="73">
         <v>3</v>
       </c>
-      <c r="J33" s="126">
+      <c r="J33" s="79">
         <f>$E$31*G33*I33</f>
         <v>168</v>
       </c>
       <c r="K33" s="44"/>
       <c r="L33" s="23"/>
       <c r="M33" s="8"/>
-      <c r="N33" s="110"/>
-      <c r="O33" s="107">
+      <c r="N33" s="102"/>
+      <c r="O33" s="97">
         <f>E40</f>
         <v>0</v>
       </c>
@@ -2922,15 +2922,15 @@
       </c>
     </row>
     <row r="34" spans="1:23" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="106"/>
-      <c r="B34" s="82"/>
-      <c r="C34" s="84" t="s">
+      <c r="A34" s="108"/>
+      <c r="B34" s="100"/>
+      <c r="C34" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="D34" s="86" t="s">
+      <c r="D34" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="78">
+      <c r="E34" s="86">
         <v>8</v>
       </c>
       <c r="F34" s="22" t="s">
@@ -2945,25 +2945,25 @@
       <c r="I34" s="73">
         <v>2</v>
       </c>
-      <c r="J34" s="126">
+      <c r="J34" s="79">
         <f>$E$34*G34*I34</f>
         <v>160</v>
       </c>
       <c r="K34" s="44"/>
       <c r="L34" s="23"/>
       <c r="M34" s="8"/>
-      <c r="N34" s="111"/>
-      <c r="O34" s="108"/>
+      <c r="N34" s="103"/>
+      <c r="O34" s="105"/>
       <c r="P34" s="48"/>
       <c r="Q34" s="23"/>
       <c r="R34" s="46"/>
     </row>
     <row r="35" spans="1:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="106"/>
-      <c r="B35" s="82"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="80"/>
+      <c r="A35" s="108"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="88"/>
       <c r="F35" s="21" t="s">
         <v>121</v>
       </c>
@@ -2976,15 +2976,15 @@
       <c r="I35" s="73">
         <v>4</v>
       </c>
-      <c r="J35" s="126">
+      <c r="J35" s="79">
         <f>$E$34*G35*I35</f>
         <v>224</v>
       </c>
       <c r="K35" s="44"/>
       <c r="L35" s="23"/>
       <c r="M35" s="8"/>
-      <c r="N35" s="111"/>
-      <c r="O35" s="108"/>
+      <c r="N35" s="103"/>
+      <c r="O35" s="105"/>
       <c r="P35" s="48">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -2996,8 +2996,8 @@
       </c>
     </row>
     <row r="36" spans="1:23" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="106"/>
-      <c r="B36" s="82"/>
+      <c r="A36" s="108"/>
+      <c r="B36" s="100"/>
       <c r="C36" s="44" t="s">
         <v>96</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>110</v>
       </c>
       <c r="E36" s="7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F36" s="22" t="s">
         <v>123</v>
@@ -3017,17 +3017,17 @@
         <v>91</v>
       </c>
       <c r="I36" s="73">
-        <v>10</v>
-      </c>
-      <c r="J36" s="126">
+        <v>9</v>
+      </c>
+      <c r="J36" s="79">
         <f>$E$36*G36*I36</f>
-        <v>800</v>
+        <v>576</v>
       </c>
       <c r="K36" s="44"/>
       <c r="L36" s="23"/>
       <c r="M36" s="8"/>
-      <c r="N36" s="111"/>
-      <c r="O36" s="108"/>
+      <c r="N36" s="103"/>
+      <c r="O36" s="105"/>
       <c r="P36" s="48">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -3039,15 +3039,15 @@
       </c>
     </row>
     <row r="37" spans="1:23" ht="47.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="106"/>
-      <c r="B37" s="82"/>
-      <c r="C37" s="84" t="s">
+      <c r="A37" s="108"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="86" t="s">
+      <c r="D37" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="78">
+      <c r="E37" s="86">
         <v>7</v>
       </c>
       <c r="F37" s="22" t="s">
@@ -3062,25 +3062,25 @@
       <c r="I37" s="73">
         <v>8</v>
       </c>
-      <c r="J37" s="126">
+      <c r="J37" s="79">
         <f>$E$37*G37*I37</f>
         <v>280</v>
       </c>
       <c r="K37" s="44"/>
       <c r="L37" s="23"/>
       <c r="M37" s="8"/>
-      <c r="N37" s="111"/>
-      <c r="O37" s="108"/>
+      <c r="N37" s="103"/>
+      <c r="O37" s="105"/>
       <c r="P37" s="48"/>
       <c r="Q37" s="23"/>
       <c r="R37" s="46"/>
     </row>
     <row r="38" spans="1:23" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="106"/>
-      <c r="B38" s="82"/>
-      <c r="C38" s="85"/>
-      <c r="D38" s="88"/>
-      <c r="E38" s="80"/>
+      <c r="A38" s="108"/>
+      <c r="B38" s="100"/>
+      <c r="C38" s="81"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="88"/>
       <c r="F38" s="21" t="s">
         <v>124</v>
       </c>
@@ -3093,29 +3093,29 @@
       <c r="I38" s="73">
         <v>4</v>
       </c>
-      <c r="J38" s="126">
+      <c r="J38" s="79">
         <f>$E$37*G38*I38</f>
         <v>168</v>
       </c>
       <c r="K38" s="44"/>
       <c r="L38" s="23"/>
       <c r="M38" s="8"/>
-      <c r="N38" s="111"/>
-      <c r="O38" s="108"/>
+      <c r="N38" s="103"/>
+      <c r="O38" s="105"/>
       <c r="P38" s="48"/>
       <c r="Q38" s="23"/>
       <c r="R38" s="46"/>
     </row>
     <row r="39" spans="1:23" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="106"/>
-      <c r="B39" s="82"/>
-      <c r="C39" s="75" t="s">
+      <c r="A39" s="108"/>
+      <c r="B39" s="100"/>
+      <c r="C39" s="110" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="75" t="s">
+      <c r="D39" s="110" t="s">
         <v>112</v>
       </c>
-      <c r="E39" s="78">
+      <c r="E39" s="86">
         <v>10</v>
       </c>
       <c r="F39" s="22" t="s">
@@ -3130,15 +3130,15 @@
       <c r="I39" s="73">
         <v>1</v>
       </c>
-      <c r="J39" s="126">
+      <c r="J39" s="79">
         <f>$E$39*G39*I39</f>
         <v>80</v>
       </c>
       <c r="K39" s="44"/>
       <c r="L39" s="23"/>
       <c r="M39" s="8"/>
-      <c r="N39" s="112"/>
-      <c r="O39" s="109"/>
+      <c r="N39" s="104"/>
+      <c r="O39" s="106"/>
       <c r="P39" s="48">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -3150,11 +3150,11 @@
       </c>
     </row>
     <row r="40" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="106"/>
-      <c r="B40" s="82"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="79"/>
+      <c r="A40" s="108"/>
+      <c r="B40" s="100"/>
+      <c r="C40" s="126"/>
+      <c r="D40" s="126"/>
+      <c r="E40" s="87"/>
       <c r="F40" s="22" t="s">
         <v>127</v>
       </c>
@@ -3167,15 +3167,15 @@
       <c r="I40" s="73">
         <v>4</v>
       </c>
-      <c r="J40" s="126">
+      <c r="J40" s="79">
         <f>$E$39*G40*I40</f>
         <v>320</v>
       </c>
       <c r="K40" s="44"/>
       <c r="L40" s="23"/>
       <c r="M40" s="8"/>
-      <c r="N40" s="110"/>
-      <c r="O40" s="107">
+      <c r="N40" s="102"/>
+      <c r="O40" s="97">
         <f>E40</f>
         <v>0</v>
       </c>
@@ -3190,11 +3190,11 @@
       </c>
     </row>
     <row r="41" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="106"/>
-      <c r="B41" s="82"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="79"/>
+      <c r="A41" s="108"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="126"/>
+      <c r="D41" s="126"/>
+      <c r="E41" s="87"/>
       <c r="F41" s="23" t="s">
         <v>128</v>
       </c>
@@ -3207,15 +3207,15 @@
       <c r="I41" s="73">
         <v>5</v>
       </c>
-      <c r="J41" s="126">
+      <c r="J41" s="79">
         <f>$E$39*G41*I41</f>
         <v>350</v>
       </c>
       <c r="K41" s="44"/>
       <c r="L41" s="23"/>
       <c r="M41" s="8"/>
-      <c r="N41" s="111"/>
-      <c r="O41" s="115"/>
+      <c r="N41" s="103"/>
+      <c r="O41" s="98"/>
       <c r="P41" s="48">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -3227,11 +3227,11 @@
       </c>
     </row>
     <row r="42" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="106"/>
-      <c r="B42" s="83"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="80"/>
+      <c r="A42" s="108"/>
+      <c r="B42" s="101"/>
+      <c r="C42" s="111"/>
+      <c r="D42" s="111"/>
+      <c r="E42" s="88"/>
       <c r="F42" s="23" t="s">
         <v>130</v>
       </c>
@@ -3244,15 +3244,15 @@
       <c r="I42" s="73">
         <v>5</v>
       </c>
-      <c r="J42" s="126">
+      <c r="J42" s="79">
         <f>$E$39*G42*I42</f>
         <v>400</v>
       </c>
       <c r="K42" s="44"/>
       <c r="L42" s="23"/>
       <c r="M42" s="8"/>
-      <c r="N42" s="111"/>
-      <c r="O42" s="115"/>
+      <c r="N42" s="103"/>
+      <c r="O42" s="98"/>
       <c r="P42" s="48">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -3264,21 +3264,21 @@
       </c>
     </row>
     <row r="43" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="105"/>
-      <c r="B43" s="81"/>
-      <c r="C43" s="86"/>
-      <c r="D43" s="86"/>
-      <c r="E43" s="107"/>
+      <c r="A43" s="107"/>
+      <c r="B43" s="99"/>
+      <c r="C43" s="91"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="97"/>
       <c r="F43" s="23"/>
-      <c r="G43" s="107"/>
+      <c r="G43" s="97"/>
       <c r="H43" s="23"/>
       <c r="I43" s="50"/>
       <c r="J43" s="43"/>
       <c r="K43" s="44"/>
       <c r="L43" s="23"/>
       <c r="M43" s="8"/>
-      <c r="N43" s="110"/>
-      <c r="O43" s="107">
+      <c r="N43" s="102"/>
+      <c r="O43" s="97">
         <f>E43</f>
         <v>0</v>
       </c>
@@ -3293,21 +3293,21 @@
       </c>
     </row>
     <row r="44" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="106"/>
-      <c r="B44" s="82"/>
-      <c r="C44" s="87"/>
-      <c r="D44" s="87"/>
-      <c r="E44" s="108"/>
+      <c r="A44" s="108"/>
+      <c r="B44" s="100"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="105"/>
       <c r="F44" s="21"/>
-      <c r="G44" s="108"/>
+      <c r="G44" s="105"/>
       <c r="H44" s="23"/>
       <c r="I44" s="50"/>
       <c r="J44" s="43"/>
       <c r="K44" s="44"/>
       <c r="L44" s="23"/>
       <c r="M44" s="8"/>
-      <c r="N44" s="111"/>
-      <c r="O44" s="115"/>
+      <c r="N44" s="103"/>
+      <c r="O44" s="98"/>
       <c r="P44" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3319,21 +3319,21 @@
       </c>
     </row>
     <row r="45" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="106"/>
-      <c r="B45" s="82"/>
-      <c r="C45" s="87"/>
-      <c r="D45" s="87"/>
-      <c r="E45" s="108"/>
+      <c r="A45" s="108"/>
+      <c r="B45" s="100"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
+      <c r="E45" s="105"/>
       <c r="F45" s="21"/>
-      <c r="G45" s="108"/>
+      <c r="G45" s="105"/>
       <c r="H45" s="23"/>
       <c r="I45" s="50"/>
       <c r="J45" s="43"/>
       <c r="K45" s="44"/>
       <c r="L45" s="23"/>
       <c r="M45" s="8"/>
-      <c r="N45" s="111"/>
-      <c r="O45" s="115"/>
+      <c r="N45" s="103"/>
+      <c r="O45" s="98"/>
       <c r="P45" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3345,21 +3345,21 @@
       </c>
     </row>
     <row r="46" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="106"/>
-      <c r="B46" s="82"/>
-      <c r="C46" s="87"/>
-      <c r="D46" s="87"/>
-      <c r="E46" s="108"/>
+      <c r="A46" s="108"/>
+      <c r="B46" s="100"/>
+      <c r="C46" s="92"/>
+      <c r="D46" s="92"/>
+      <c r="E46" s="105"/>
       <c r="F46" s="21"/>
-      <c r="G46" s="108"/>
+      <c r="G46" s="105"/>
       <c r="H46" s="23"/>
       <c r="I46" s="50"/>
       <c r="J46" s="43"/>
       <c r="K46" s="44"/>
       <c r="L46" s="23"/>
       <c r="M46" s="8"/>
-      <c r="N46" s="111"/>
-      <c r="O46" s="115"/>
+      <c r="N46" s="103"/>
+      <c r="O46" s="98"/>
       <c r="P46" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3371,21 +3371,21 @@
       </c>
     </row>
     <row r="47" spans="1:23" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="114"/>
-      <c r="B47" s="83"/>
-      <c r="C47" s="88"/>
-      <c r="D47" s="88"/>
-      <c r="E47" s="109"/>
+      <c r="A47" s="109"/>
+      <c r="B47" s="101"/>
+      <c r="C47" s="93"/>
+      <c r="D47" s="93"/>
+      <c r="E47" s="106"/>
       <c r="F47" s="23"/>
-      <c r="G47" s="109"/>
+      <c r="G47" s="106"/>
       <c r="H47" s="23"/>
       <c r="I47" s="50"/>
       <c r="J47" s="43"/>
       <c r="K47" s="44"/>
       <c r="L47" s="23"/>
       <c r="M47" s="8"/>
-      <c r="N47" s="112"/>
-      <c r="O47" s="113"/>
+      <c r="N47" s="104"/>
+      <c r="O47" s="85"/>
       <c r="P47" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3834,53 +3834,14 @@
     <row r="451" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="O43:O47"/>
-    <mergeCell ref="B21:B30"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="N43:N47"/>
-    <mergeCell ref="O33:O39"/>
-    <mergeCell ref="N40:N42"/>
-    <mergeCell ref="O40:O42"/>
-    <mergeCell ref="N33:N39"/>
-    <mergeCell ref="O21:O24"/>
-    <mergeCell ref="A43:A47"/>
-    <mergeCell ref="C43:C47"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="E43:E47"/>
-    <mergeCell ref="G43:G47"/>
-    <mergeCell ref="A33:A42"/>
-    <mergeCell ref="P21:P24"/>
-    <mergeCell ref="N26:N30"/>
-    <mergeCell ref="O26:O30"/>
-    <mergeCell ref="P26:P30"/>
-    <mergeCell ref="N21:N24"/>
-    <mergeCell ref="A21:A30"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="H2:L2"/>
@@ -3897,11 +3858,36 @@
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="B6:B20"/>
+    <mergeCell ref="A33:A42"/>
+    <mergeCell ref="P21:P24"/>
+    <mergeCell ref="N26:N30"/>
+    <mergeCell ref="O26:O30"/>
+    <mergeCell ref="P26:P30"/>
+    <mergeCell ref="N21:N24"/>
+    <mergeCell ref="A21:A30"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="C43:C47"/>
+    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="E43:E47"/>
+    <mergeCell ref="G43:G47"/>
+    <mergeCell ref="O43:O47"/>
+    <mergeCell ref="B21:B30"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="N43:N47"/>
+    <mergeCell ref="O33:O39"/>
+    <mergeCell ref="N40:N42"/>
+    <mergeCell ref="O40:O42"/>
+    <mergeCell ref="N33:N39"/>
+    <mergeCell ref="O21:O24"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="E29:E30"/>
     <mergeCell ref="D39:D42"/>
@@ -3909,14 +3895,28 @@
     <mergeCell ref="E39:E42"/>
     <mergeCell ref="B33:B42"/>
     <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="J6:J8 J10:J11 J13:J47">
     <cfRule type="colorScale" priority="89">
@@ -3963,7 +3963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="145" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -4134,9 +4134,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4305,27 +4308,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{321A4371-70D3-4670-B9DE-51C73593625E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D99D69-C41B-42E2-B319-512FDE30DA9C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b4c971ed-d55e-45d5-823f-e5f0a4d5378a"/>
-    <ds:schemaRef ds:uri="fb007535-a6a4-4ea0-86da-29f43c46b391"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4350,9 +4341,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D99D69-C41B-42E2-B319-512FDE30DA9C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{321A4371-70D3-4670-B9DE-51C73593625E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b4c971ed-d55e-45d5-823f-e5f0a4d5378a"/>
+    <ds:schemaRef ds:uri="fb007535-a6a4-4ea0-86da-29f43c46b391"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>